<commit_message>
Fixed working for all notes
</commit_message>
<xml_diff>
--- a/English vocabulary.xlsx
+++ b/English vocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asia\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008852F5-E8AB-4195-8E48-8068E46213B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB7BF2D-CB55-463F-A2B0-C1C991281A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Advanced vocabulary" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="305">
   <si>
     <t>Lp.</t>
   </si>
@@ -73,115 +73,58 @@
     </r>
   </si>
   <si>
-    <t>Meticulous</t>
-  </si>
-  <si>
     <t>skrupulatny, drobiazgowy</t>
   </si>
   <si>
-    <t>Plausible</t>
-  </si>
-  <si>
     <t>wiarygodny, możliwy</t>
   </si>
   <si>
-    <t>Deteriorate</t>
-  </si>
-  <si>
     <t>pogarszać się</t>
   </si>
   <si>
-    <t>Scrutinize</t>
-  </si>
-  <si>
     <t>dokładnie badać</t>
   </si>
   <si>
-    <t>Impartial</t>
-  </si>
-  <si>
     <t>bezstronny</t>
   </si>
   <si>
-    <t>Allegation</t>
-  </si>
-  <si>
     <t>zarzut, oskarżenie</t>
   </si>
   <si>
-    <t>Feasible</t>
-  </si>
-  <si>
     <t>wykonalny, możliwy do zrealizowania</t>
   </si>
   <si>
-    <t>Notion</t>
-  </si>
-  <si>
     <t>pojęcie, wyobrażenie</t>
   </si>
   <si>
-    <t>Resilient</t>
-  </si>
-  <si>
     <t>odporny, wytrzymały</t>
   </si>
   <si>
-    <t>Ambiguous</t>
-  </si>
-  <si>
     <t>dwuznaczny, niejednoznaczny</t>
   </si>
   <si>
-    <t>Convey</t>
-  </si>
-  <si>
     <t>przekazywać, komunikować</t>
   </si>
   <si>
-    <t>Discrepancy</t>
-  </si>
-  <si>
     <t>rozbieżność, niezgodność</t>
   </si>
   <si>
-    <t>Exacerbate</t>
-  </si>
-  <si>
     <t>pogarszać, zaostrzać</t>
   </si>
   <si>
-    <t>Ubiquitous</t>
-  </si>
-  <si>
     <t>wszechobecny</t>
   </si>
   <si>
-    <t>Inevitable</t>
-  </si>
-  <si>
     <t>nieunikniony</t>
   </si>
   <si>
-    <t>Reiterate</t>
-  </si>
-  <si>
     <t>powtarzać, podkreślać ponownie</t>
   </si>
   <si>
-    <t>Substantiate</t>
-  </si>
-  <si>
     <t>udowodnić, potwierdzić</t>
   </si>
   <si>
-    <t>Viable</t>
-  </si>
-  <si>
     <t>realny, wykonalny, rentowny</t>
-  </si>
-  <si>
-    <t>Tentative</t>
   </si>
   <si>
     <t>niepewny, wstępny</t>
@@ -733,12 +676,789 @@
       <t xml:space="preserve"> date for the meeting, but it may change.</t>
     </r>
   </si>
+  <si>
+    <t>meticulous</t>
+  </si>
+  <si>
+    <t>plausible</t>
+  </si>
+  <si>
+    <t>deteriorate</t>
+  </si>
+  <si>
+    <t>scrutinize</t>
+  </si>
+  <si>
+    <t>impartial</t>
+  </si>
+  <si>
+    <t>allegation</t>
+  </si>
+  <si>
+    <t>feasible</t>
+  </si>
+  <si>
+    <t>notion</t>
+  </si>
+  <si>
+    <t>resilient</t>
+  </si>
+  <si>
+    <t>ambiguous</t>
+  </si>
+  <si>
+    <t>convey</t>
+  </si>
+  <si>
+    <t>discrepancy</t>
+  </si>
+  <si>
+    <t>exacerbate</t>
+  </si>
+  <si>
+    <t>ubiquitous</t>
+  </si>
+  <si>
+    <t>inevitable</t>
+  </si>
+  <si>
+    <t>reiterate</t>
+  </si>
+  <si>
+    <t>substantiate</t>
+  </si>
+  <si>
+    <t>viable</t>
+  </si>
+  <si>
+    <t>tentative</t>
+  </si>
+  <si>
+    <t>desensitization</t>
+  </si>
+  <si>
+    <t>odczulanie</t>
+  </si>
+  <si>
+    <t>lightheadedness</t>
+  </si>
+  <si>
+    <t>lightheaded</t>
+  </si>
+  <si>
+    <t>hotheaded</t>
+  </si>
+  <si>
+    <t>high-handedness</t>
+  </si>
+  <si>
+    <t>bigheaded</t>
+  </si>
+  <si>
+    <t>hives</t>
+  </si>
+  <si>
+    <t>pokrzywka</t>
+  </si>
+  <si>
+    <t>porywczy, w gorącej wodzie kąpany</t>
+  </si>
+  <si>
+    <t>despotyczność</t>
+  </si>
+  <si>
+    <t>zarozumiały</t>
+  </si>
+  <si>
+    <t>decline</t>
+  </si>
+  <si>
+    <t>question mark about/over sth</t>
+  </si>
+  <si>
+    <t>isolated pockets</t>
+  </si>
+  <si>
+    <t>take sth for granted</t>
+  </si>
+  <si>
+    <t>oblivious</t>
+  </si>
+  <si>
+    <t>shrewd</t>
+  </si>
+  <si>
+    <t>daft</t>
+  </si>
+  <si>
+    <t>dim</t>
+  </si>
+  <si>
+    <t>thick</t>
+  </si>
+  <si>
+    <t>cunning</t>
+  </si>
+  <si>
+    <t>crafty</t>
+  </si>
+  <si>
+    <t>sly</t>
+  </si>
+  <si>
+    <t>wound up</t>
+  </si>
+  <si>
+    <t>down-to-earth</t>
+  </si>
+  <si>
+    <t>worked-up</t>
+  </si>
+  <si>
+    <t>even-tempered</t>
+  </si>
+  <si>
+    <t>laid-back</t>
+  </si>
+  <si>
+    <t>ill-mannered</t>
+  </si>
+  <si>
+    <t>discourteous</t>
+  </si>
+  <si>
+    <t>sincere</t>
+  </si>
+  <si>
+    <t>thrifty</t>
+  </si>
+  <si>
+    <t>economical</t>
+  </si>
+  <si>
+    <t>self-assured</t>
+  </si>
+  <si>
+    <t>unconventional</t>
+  </si>
+  <si>
+    <t>frank</t>
+  </si>
+  <si>
+    <t>enquiring</t>
+  </si>
+  <si>
+    <t>obstinate</t>
+  </si>
+  <si>
+    <t>pig-headed</t>
+  </si>
+  <si>
+    <t>stingy</t>
+  </si>
+  <si>
+    <t>miserly</t>
+  </si>
+  <si>
+    <t>full of oneself</t>
+  </si>
+  <si>
+    <t>peculiar</t>
+  </si>
+  <si>
+    <t>to be blunt</t>
+  </si>
+  <si>
+    <t>abrupt</t>
+  </si>
+  <si>
+    <t>brusque</t>
+  </si>
+  <si>
+    <t>curt</t>
+  </si>
+  <si>
+    <t>unprincipled</t>
+  </si>
+  <si>
+    <t>inquisitive</t>
+  </si>
+  <si>
+    <t>nosy</t>
+  </si>
+  <si>
+    <t>pushy</t>
+  </si>
+  <si>
+    <t>effusive</t>
+  </si>
+  <si>
+    <t>excitable</t>
+  </si>
+  <si>
+    <t>zanik, spadek</t>
+  </si>
+  <si>
+    <t>bystry, sprytny</t>
+  </si>
+  <si>
+    <t>durny, głupi, niemądry</t>
+  </si>
+  <si>
+    <t>ciemny, nierozumiejący</t>
+  </si>
+  <si>
+    <t>tępy, ociężały umysłowo</t>
+  </si>
+  <si>
+    <t>chytry, przebiegły, cwany</t>
+  </si>
+  <si>
+    <t>chytry, przebiegły</t>
+  </si>
+  <si>
+    <t>spięty, nerwowy, podekscytowany</t>
+  </si>
+  <si>
+    <t>praktyczny, twardo stąpający po ziemii</t>
+  </si>
+  <si>
+    <t>zmartwiony, podekscytowany</t>
+  </si>
+  <si>
+    <t>towarzyski</t>
+  </si>
+  <si>
+    <t>kłótliwy, swarliwy</t>
+  </si>
+  <si>
+    <t>wyluzowany</t>
+  </si>
+  <si>
+    <t>spokojny, zrównoważony</t>
+  </si>
+  <si>
+    <t>niekulturalny, źle wychowany</t>
+  </si>
+  <si>
+    <t>niegrzeczny, nieuprzejmy</t>
+  </si>
+  <si>
+    <t>szczery, nieudawany</t>
+  </si>
+  <si>
+    <t>gospodarny, oszczędny</t>
+  </si>
+  <si>
+    <t>ekonomiczny, oszczędny</t>
+  </si>
+  <si>
+    <t>pewny siebie</t>
+  </si>
+  <si>
+    <t>nieszablonowy</t>
+  </si>
+  <si>
+    <t>szczery</t>
+  </si>
+  <si>
+    <t>badawczy, doceikliwy</t>
+  </si>
+  <si>
+    <t>zawzięty, uparty, uporczywy</t>
+  </si>
+  <si>
+    <t>uparty jak osioł</t>
+  </si>
+  <si>
+    <t>skąpy</t>
+  </si>
+  <si>
+    <t>egoistyczny, zarozumiały</t>
+  </si>
+  <si>
+    <t>dziwny, osobliwy</t>
+  </si>
+  <si>
+    <t>mówić bez ogródek</t>
+  </si>
+  <si>
+    <t>obcesowy, szorstki, opryskliwy</t>
+  </si>
+  <si>
+    <t>szorstki, oschły, zbywający</t>
+  </si>
+  <si>
+    <t>pozbawiony skrupułów</t>
+  </si>
+  <si>
+    <t>dociekliwy, ciekawski</t>
+  </si>
+  <si>
+    <t>niedyskretny, wścibski</t>
+  </si>
+  <si>
+    <t>natretny, nachalny</t>
+  </si>
+  <si>
+    <t>impulsywny, porywczy</t>
+  </si>
+  <si>
+    <t>wylewny, górnolotny</t>
+  </si>
+  <si>
+    <t>pobudliwy, wrażliwy na bodźce</t>
+  </si>
+  <si>
+    <t>taciturn</t>
+  </si>
+  <si>
+    <t>outgoing</t>
+  </si>
+  <si>
+    <t>diffident</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>aloof</t>
+  </si>
+  <si>
+    <t>haughty</t>
+  </si>
+  <si>
+    <t>disdainful</t>
+  </si>
+  <si>
+    <t>unapproachable</t>
+  </si>
+  <si>
+    <t>conceited</t>
+  </si>
+  <si>
+    <t>self-important</t>
+  </si>
+  <si>
+    <t>gullible</t>
+  </si>
+  <si>
+    <t>conscientious</t>
+  </si>
+  <si>
+    <t>restless</t>
+  </si>
+  <si>
+    <t>skrępowany, nieśmiały, zakłopotany</t>
+  </si>
+  <si>
+    <t>małomówny, mrukliwy</t>
+  </si>
+  <si>
+    <t>otwary, towarzyski</t>
+  </si>
+  <si>
+    <t>niesmiały, niepewny siebie</t>
+  </si>
+  <si>
+    <t>powściągliwy, skryty</t>
+  </si>
+  <si>
+    <t>powściągliwy, z dystansem</t>
+  </si>
+  <si>
+    <t>pogardliwy, lekceważący</t>
+  </si>
+  <si>
+    <t>nieprzystępny</t>
+  </si>
+  <si>
+    <t>posiadający, wysokie mniemanie o sobie</t>
+  </si>
+  <si>
+    <t>łatwowierny</t>
+  </si>
+  <si>
+    <t>niespopkojny, nerwowy</t>
+  </si>
+  <si>
+    <t>uczucie pustki w głowie, zawroty głowy</t>
+  </si>
+  <si>
+    <t>oszołomiony, mający zawroty głowy</t>
+  </si>
+  <si>
+    <t>gregarious</t>
+  </si>
+  <si>
+    <t>quarrelsome</t>
+  </si>
+  <si>
+    <t>tight-fisted</t>
+  </si>
+  <si>
+    <t>impetuous</t>
+  </si>
+  <si>
+    <t>self-conscious</t>
+  </si>
+  <si>
+    <t>sumienny, skrupulatny</t>
+  </si>
+  <si>
+    <t>butny, dumny, wyniosły</t>
+  </si>
+  <si>
+    <t>The doctor recommended desensitization therapy for her allergies.</t>
+  </si>
+  <si>
+    <t>After eating strawberries, he broke out in hives.</t>
+  </si>
+  <si>
+    <t>She experienced lightheadedness after standing up too quickly.</t>
+  </si>
+  <si>
+    <t>I felt lightheaded in the heat.</t>
+  </si>
+  <si>
+    <t>He’s too hotheaded to negotiate calmly.</t>
+  </si>
+  <si>
+    <t>The manager’s high-handedness made everyone uncomfortable.</t>
+  </si>
+  <si>
+    <t>Don’t get bigheaded after one success.</t>
+  </si>
+  <si>
+    <t>There’s been a steady decline in sales this year.</t>
+  </si>
+  <si>
+    <t>There’s still a question mark over his future at the company.</t>
+  </si>
+  <si>
+    <t>There are isolated pockets of resistance in the area.</t>
+  </si>
+  <si>
+    <t>Don’t take your health for granted.</t>
+  </si>
+  <si>
+    <t>He walked into the street, oblivious to the traffic.</t>
+  </si>
+  <si>
+    <t>She’s a shrewd businesswoman.</t>
+  </si>
+  <si>
+    <t>What a daft idea!</t>
+  </si>
+  <si>
+    <t>He’s nice, but a bit dim.</t>
+  </si>
+  <si>
+    <t>How can you be so thick?</t>
+  </si>
+  <si>
+    <t>The cunning fox tricked the farmer.</t>
+  </si>
+  <si>
+    <t>She’s crafty when it comes to getting what she wants.</t>
+  </si>
+  <si>
+    <t>He gave me a sly smile.</t>
+  </si>
+  <si>
+    <t>I’m too wound up to sleep.</t>
+  </si>
+  <si>
+    <t>She’s very down-to-earth and practical.</t>
+  </si>
+  <si>
+    <t>Don’t get so worked-up about it.</t>
+  </si>
+  <si>
+    <t>He’s gregarious and loves parties.</t>
+  </si>
+  <si>
+    <t>They’re a quarrelsome couple.</t>
+  </si>
+  <si>
+    <t>He’s calm and even-tempered under pressure.</t>
+  </si>
+  <si>
+    <t>She has a laid-back attitude to life.</t>
+  </si>
+  <si>
+    <t>The child was rude and ill-mannered.</t>
+  </si>
+  <si>
+    <t>It was discourteous of him to interrupt.</t>
+  </si>
+  <si>
+    <t>I believe his apology was sincere.</t>
+  </si>
+  <si>
+    <t>She’s thrifty and never wastes money.</t>
+  </si>
+  <si>
+    <t>This car is very economical on fuel.</t>
+  </si>
+  <si>
+    <t>She spoke in a self-assured voice.</t>
+  </si>
+  <si>
+    <t>His methods are unconventional but effective.</t>
+  </si>
+  <si>
+    <t>Let me be frank with you.</t>
+  </si>
+  <si>
+    <t>She had an enquiring mind from an early age.</t>
+  </si>
+  <si>
+    <t>He’s obstinate and refuses to change his mind.</t>
+  </si>
+  <si>
+    <t>Don’t be so pig-headed!</t>
+  </si>
+  <si>
+    <t>He’s too stingy to buy a round of drinks.</t>
+  </si>
+  <si>
+    <t>My uncle is tight-fisted with his money.</t>
+  </si>
+  <si>
+    <t>He lived a miserly life despite his wealth.</t>
+  </si>
+  <si>
+    <t>He’s so full of himself.</t>
+  </si>
+  <si>
+    <t>That’s a peculiar smell.</t>
+  </si>
+  <si>
+    <t>To be blunt, your plan won’t work.</t>
+  </si>
+  <si>
+    <t>His abrupt manner offended her.</t>
+  </si>
+  <si>
+    <t>She can be brusque at times.</t>
+  </si>
+  <si>
+    <t>His reply was curt and unfriendly.</t>
+  </si>
+  <si>
+    <t>He’s an unprincipled politician.</t>
+  </si>
+  <si>
+    <t>An inquisitive child asked endless questions.</t>
+  </si>
+  <si>
+    <t>Don’t be so nosy!</t>
+  </si>
+  <si>
+    <t>He’s a pushy salesman.</t>
+  </si>
+  <si>
+    <t>He made an impetuous decision without thinking.</t>
+  </si>
+  <si>
+    <t>She gave him an effusive welcome.</t>
+  </si>
+  <si>
+    <t>The dog is very excitable around strangers.</t>
+  </si>
+  <si>
+    <t>He felt self-conscious about his accent.</t>
+  </si>
+  <si>
+    <t>He’s a taciturn man who rarely speaks.</t>
+  </si>
+  <si>
+    <t>She’s outgoing and makes friends easily.</t>
+  </si>
+  <si>
+    <t>He’s diffident in large groups</t>
+  </si>
+  <si>
+    <t>She’s quite reserved with strangers.</t>
+  </si>
+  <si>
+    <t>He stayed aloof from the argument.</t>
+  </si>
+  <si>
+    <t>She looked at me with a haughty expression.</t>
+  </si>
+  <si>
+    <t>He gave a disdainful laugh.</t>
+  </si>
+  <si>
+    <t>The boss seemed unapproachable at the meeting.</t>
+  </si>
+  <si>
+    <t>He’s too conceited to admit he’s wrong.</t>
+  </si>
+  <si>
+    <t>She’s so self-important since her promotion.</t>
+  </si>
+  <si>
+    <t>Don’t be so gullible, it’s a scam.</t>
+  </si>
+  <si>
+    <t>She’s a conscientious student.</t>
+  </si>
+  <si>
+    <t>I felt restless before the exam.</t>
+  </si>
+  <si>
+    <t>wątpliwości dotyczące czegoś</t>
+  </si>
+  <si>
+    <t>odosobnione skupiska/enklawy</t>
+  </si>
+  <si>
+    <t>brać coś za pewnik</t>
+  </si>
+  <si>
+    <t>nieświadomy, niezdający sobie sprawy</t>
+  </si>
+  <si>
+    <t>countryside</t>
+  </si>
+  <si>
+    <t>obszar wiejski, głównie pod uprawę</t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>wieś, wioska</t>
+  </si>
+  <si>
+    <t>sagebruch, artemisia</t>
+  </si>
+  <si>
+    <t>bylica</t>
+  </si>
+  <si>
+    <t>over-the-counter (OTC)</t>
+  </si>
+  <si>
+    <t>dostępny bez recepty</t>
+  </si>
+  <si>
+    <t>air rifle, air gun</t>
+  </si>
+  <si>
+    <t>wiatrówka (pistolet)</t>
+  </si>
+  <si>
+    <t>windcheater</t>
+  </si>
+  <si>
+    <t>wiatrówka (kurtka)</t>
+  </si>
+  <si>
+    <t>steadily</t>
+  </si>
+  <si>
+    <t>stopniowo, równomiernie</t>
+  </si>
+  <si>
+    <t>break in</t>
+  </si>
+  <si>
+    <t>włamać się</t>
+  </si>
+  <si>
+    <t>pollinate</t>
+  </si>
+  <si>
+    <t>zapylić</t>
+  </si>
+  <si>
+    <t>seed</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>meadow</t>
+  </si>
+  <si>
+    <t>łąka</t>
+  </si>
+  <si>
+    <t>siać</t>
+  </si>
+  <si>
+    <t>sadzić</t>
+  </si>
+  <si>
+    <t>humble</t>
+  </si>
+  <si>
+    <t>pinchpenny</t>
+  </si>
+  <si>
+    <t>money grabber</t>
+  </si>
+  <si>
+    <t>pokorny skromny</t>
+  </si>
+  <si>
+    <t>zachłanny</t>
+  </si>
+  <si>
+    <t>We spent the weekend in the countryside.</t>
+  </si>
+  <si>
+    <t>She grew up in a small village in the mountains.</t>
+  </si>
+  <si>
+    <t>Sagebrush grows abundantly in this desert region.</t>
+  </si>
+  <si>
+    <t>You can buy these painkillers over the counter.</t>
+  </si>
+  <si>
+    <t>He learned to shoot with an air rifle at the age of ten.</t>
+  </si>
+  <si>
+    <t>She put on a windcheater before going for a run.</t>
+  </si>
+  <si>
+    <t>The rain fell steadily all night.</t>
+  </si>
+  <si>
+    <t>Someone tried to break in last night.</t>
+  </si>
+  <si>
+    <t>Bees help pollinate flowers.</t>
+  </si>
+  <si>
+    <t>We will plant tomatoes in the garden.</t>
+  </si>
+  <si>
+    <t>The cows were grazing in the meadow.</t>
+  </si>
+  <si>
+    <t>He remained humble despite his success.</t>
+  </si>
+  <si>
+    <t>Don’t be such a pinchpenny—just buy the ticket!</t>
+  </si>
+  <si>
+    <t>The landlord is a real money grabber.</t>
+  </si>
+  <si>
+    <t>Farmers seed their fields in early spring.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,8 +1493,30 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -784,6 +1526,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,11 +1593,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1102,14 +1895,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E352"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="21.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="1" customWidth="1"/>
     <col min="3" max="3" width="34.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="123.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
@@ -1129,740 +1922,1580 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B48" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B51" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B52" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="11">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B53" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E53" s="11"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="11">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="B54" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E54" s="11"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="11">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="B55" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E55" s="11"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="11">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B56" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E56" s="11"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="11">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="B57" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E57" s="11"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="11">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="B58" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="E58" s="11"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="11">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="B59" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E59" s="11"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="11">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="B60" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E60" s="11"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="11">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="B61" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E61" s="11"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="11">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="B62" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62" s="11"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="11">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="B63" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E63" s="11"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="11">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="B64" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E64" s="11"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="11">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
+      <c r="B65" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E65" s="11"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="11">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+      <c r="B66" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E66" s="11"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="11">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
+      <c r="B67" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E67" s="11"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="11">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
+      <c r="B68" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E68" s="11"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="11">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
+      <c r="B69" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="E69" s="11"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="11">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
+      <c r="B70" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E70" s="11"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="11">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
+      <c r="B71" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="E71" s="11"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="11">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
+      <c r="B72" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="E72" s="11"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="15">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
+      <c r="B73" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="E73" s="15"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="15">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
+      <c r="B74" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="E74" s="15"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="15">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
+      <c r="B75" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="E75" s="15"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="15">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
+      <c r="B76" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E76" s="15"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="15">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
+      <c r="B77" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="E77" s="15"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="15">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
+      <c r="B78" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E78" s="15"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="15">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
+      <c r="B79" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="E79" s="15"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="15">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
+      <c r="B80" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D80" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="E80" s="15"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="15">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
+      <c r="B81" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="E81" s="15"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="15">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1">
+      <c r="B82" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E82" s="15"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="15">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
+      <c r="B83" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E83" s="15"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="15">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1">
+      <c r="B84" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E84" s="15"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="15">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1">
+      <c r="B85" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E85" s="15"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="15">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1">
+      <c r="B86" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E86" s="15"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="15">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
+      <c r="B87" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E87" s="15"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="15">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
+      <c r="B88" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="E88" s="15"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="15">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1">
+      <c r="B89" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="E89" s="15"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="15">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1">
+      <c r="B90" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="E90" s="15"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="15">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1">
+      <c r="B91" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="E91" s="15"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="15">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1">
+      <c r="B92" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C92" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="E92" s="15"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="15">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="1">
+      <c r="B93" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="E93" s="15"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="18">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="1">
+      <c r="B94" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="E94" s="18"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="18">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1">
+      <c r="B95" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="E95" s="18"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="18">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="1">
+      <c r="B96" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="E96" s="18"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="18">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="1">
+      <c r="B97" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="E97" s="18"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="18">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="1">
+      <c r="B98" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="E98" s="18"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="18">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="1">
+      <c r="B99" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="E99" s="18"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="18">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1">
+      <c r="B100" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="E100" s="18"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="18">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="1">
+      <c r="B101" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="E101" s="18"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="18">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="1">
+      <c r="B102" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="E102" s="18"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="18">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B103" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="E103" s="18"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>111</v>
       </c>

</xml_diff>